<commit_message>
Changed green color for Value Bridge
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kpi_mappings.xlsx
+++ b/public/sample_uploads/investor_kpi_mappings.xlsx
@@ -267,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Investor *</t>
   </si>
@@ -299,6 +299,9 @@
     <t xml:space="preserve">Upper Threshold</t>
   </si>
   <si>
+    <t xml:space="preserve">Cumulate</t>
+  </si>
+  <si>
     <t xml:space="preserve">ABC</t>
   </si>
   <si>
@@ -315,6 +318,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
   </si>
 </sst>
 </file>
@@ -459,7 +465,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,11 +478,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -681,10 +695,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -698,11 +712,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16376" style="1" width="10.16"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -733,29 +747,32 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="n">
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>15</v>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>0</v>
@@ -763,186 +780,189 @@
       <c r="J2" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="K2" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed tests post changes to Stakeholder
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kpi_mappings.xlsx
+++ b/public/sample_uploads/investor_kpi_mappings.xlsx
@@ -269,7 +269,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t xml:space="preserve">Investor *</t>
+    <t xml:space="preserve">Stakeholder *</t>
   </si>
   <si>
     <t xml:space="preserve">Standard Kpi Name *</t>
@@ -478,7 +478,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -490,7 +490,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -698,7 +698,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>